<commit_message>
# Conclusions 17 - Learning rate 0.02 - Results - accuracies are not good - product .92% ### Conclusions going forward: - Go back to much lower learning rates - try 0.005
</commit_message>
<xml_diff>
--- a/output/17_learn_rate_0.02/full.xlsx
+++ b/output/17_learn_rate_0.02/full.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,13 +468,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.02</v>
+        <v>0.0001</v>
       </c>
       <c r="C2" t="n">
         <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="E2" t="n">
         <v>200</v>
@@ -491,40 +491,296 @@
         <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0001</v>
+        <v>0.02</v>
       </c>
       <c r="J2" t="n">
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9398000240325928</v>
+        <v>0.9652000069618225</v>
       </c>
       <c r="L2" t="n">
-        <v>0.879800021648407</v>
+        <v>0.9287999868392944</v>
       </c>
       <c r="M2" t="n">
-        <v>49.748</v>
+        <v>77.307</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0189</v>
+        <v>0.0125</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0177</v>
+        <v>0.012</v>
       </c>
       <c r="P2" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>7.0279</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.9617999792098999</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.958899974822998</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.9623000025749207</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>200</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>('tanh', 'relu')</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>100</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.9617999792098999</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.9182999730110168</v>
+      </c>
+      <c r="M3" t="n">
+        <v>43.371</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.0222</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.0212</v>
+      </c>
+      <c r="P3" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>7.2285</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.9567999839782715</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.9524999856948853</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.9546999931335449</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>200</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>('tanh', 'relu')</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>100</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="J4" t="n">
+        <v>3</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.9596999883651733</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.914900004863739</v>
+      </c>
+      <c r="M4" t="n">
+        <v>44.608</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.0215</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.0205</v>
+      </c>
+      <c r="P4" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>7.4347</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.9514999985694885</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.9526000022888184</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.9532999992370605</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E5" t="n">
+        <v>200</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>('tanh', 'relu')</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>100</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="J5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.9646999835968018</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.9246000051498413</v>
+      </c>
+      <c r="M5" t="n">
+        <v>59.611</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.0162</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.0155</v>
+      </c>
+      <c r="P5" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>7.4514</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.9596999883651733</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.9584000110626221</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.9584000110626221</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E6" t="n">
+        <v>200</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>('tanh', 'relu')</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>100</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="J6" t="n">
+        <v>5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.9589999914169312</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.9156000018119812</v>
+      </c>
+      <c r="M6" t="n">
+        <v>51.33</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.0187</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.0178</v>
+      </c>
+      <c r="P6" t="n">
         <v>7</v>
       </c>
-      <c r="Q2" t="n">
-        <v>7.1069</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0.9398000240325928</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0.9361000061035156</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0.9361000061035156</v>
+      <c r="Q6" t="n">
+        <v>7.3329</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.9570000171661377</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.9545999765396118</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.954800009727478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>